<commit_message>
updates to baseline graphs and mine supply
in metric tonnes
</commit_message>
<xml_diff>
--- a/PV_ICE/baselines/ReedsSubset/BaselineGraphs.xlsx
+++ b/PV_ICE/baselines/ReedsSubset/BaselineGraphs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmirletz\Documents\GitHub\PV_ICE\PV_ICE\baselines\ReedsSubset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243771B8-0469-475F-B209-8474D698EC76}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1163B67E-8CB1-4572-B3BE-49F7821B9ACB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-4680" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{31D47E9D-A833-4D35-B79A-EFF0E4DE6D01}"/>
+    <workbookView xWindow="20370" yWindow="-4680" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{31D47E9D-A833-4D35-B79A-EFF0E4DE6D01}"/>
   </bookViews>
   <sheets>
     <sheet name="mass per m2" sheetId="1" r:id="rId1"/>
@@ -148,11 +148,11 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -161,6 +161,15 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFD62728"/>
+      <color rgb="FF2CA02C"/>
+      <color rgb="FF1F77B4"/>
+      <color rgb="FFFF7F0E"/>
+      <color rgb="FF00BFBF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -8569,64 +8578,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>PV Evolution: Mass per module area over time</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.2073786135382862E-2"/>
+          <c:y val="3.051149687266726E-2"/>
+          <c:w val="0.86475696867005547"/>
+          <c:h val="0.86151854039929188"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -8645,9 +8609,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="00BFBF"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -8948,9 +8912,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="00B0F0"/>
+                <a:srgbClr val="FF7F0E"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -9251,9 +9215,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:srgbClr val="1F77B4"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -9554,9 +9518,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="2CA02C"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -9857,9 +9821,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:srgbClr val="D62728"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -10160,7 +10124,7 @@
         <c:axId val="664749616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="2050"/>
+          <c:max val="2030"/>
           <c:min val="2010"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -10187,10 +10151,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -10201,16 +10162,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -10243,20 +10201,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="5000"/>
-                  <a:lumOff val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -10264,21 +10208,18 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:latin typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Mass per Module m^2 (grams, hectograms, kilograms)</a:t>
+                  <a:t>Mass per m2 of module [grams | hectograms | kilograms]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -10296,16 +10237,13 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:latin typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="en-US"/>
@@ -10320,10 +10258,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -10334,16 +10269,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -10357,7 +10289,9 @@
       <c:spPr>
         <a:noFill/>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -10368,10 +10302,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.74745443739363815"/>
-          <c:y val="0.12459637902355944"/>
-          <c:w val="0.20939372499633777"/>
-          <c:h val="0.21855266196760129"/>
+          <c:x val="0.70057211203030001"/>
+          <c:y val="4.4953407888784415E-2"/>
+          <c:w val="0.24877489469934402"/>
+          <c:h val="0.26249354509180456"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -10382,7 +10316,7 @@
         <a:ln>
           <a:solidFill>
             <a:schemeClr val="bg1">
-              <a:lumMod val="50000"/>
+              <a:lumMod val="75000"/>
             </a:schemeClr>
           </a:solidFill>
         </a:ln>
@@ -10393,16 +10327,13 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:latin typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -10424,13 +10355,8 @@
     <a:solidFill>
       <a:schemeClr val="bg1"/>
     </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+    <a:ln w="28575" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -10440,7 +10366,14 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1050">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:latin typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+          <a:ea typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -16681,8 +16614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56D7BEC5-C527-4A05-96EF-71A772E43E2F}">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F2"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16691,23 +16624,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="2" t="s">
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -18264,8 +18197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0188699D-EC8B-4A24-8D21-3FBF9C878E79}">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="X3" sqref="X3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18274,19 +18207,19 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -19804,7 +19737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2886825C-AE4A-4EAF-970C-700F7CC3D78A}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>

</xml_diff>